<commit_message>
Changes to CT tables to allow GEEGLM
</commit_message>
<xml_diff>
--- a/validated/src/main/resources/analysis-r/experiment-results-for-paper/raw-data-and-plots.xlsx
+++ b/validated/src/main/resources/analysis-r/experiment-results-for-paper/raw-data-and-plots.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsd4/Desktop/exp-res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsd4/OneDrive/cs/PhD/code/population-model/validated/src/main/resources/analysis-r/experiment-results-for-paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Runtimes" sheetId="3" r:id="rId3"/>
     <sheet name="CT Init" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -703,11 +703,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1291211296"/>
-        <c:axId val="-1291213072"/>
+        <c:axId val="-903293616"/>
+        <c:axId val="-903290912"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1291211296"/>
+        <c:axId val="-903293616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.7E7"/>
@@ -766,7 +766,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1291213072"/>
+        <c:crossAx val="-903290912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -829,7 +829,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1291213072"/>
+        <c:axId val="-903290912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -887,7 +887,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1291211296"/>
+        <c:crossAx val="-903293616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="0.5"/>
@@ -1319,11 +1319,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1309409888"/>
-        <c:axId val="-1315991296"/>
+        <c:axId val="-844851008"/>
+        <c:axId val="-844847248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1309409888"/>
+        <c:axId val="-844851008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.7E7"/>
@@ -1382,7 +1382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1315991296"/>
+        <c:crossAx val="-844847248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1453,7 +1453,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1315991296"/>
+        <c:axId val="-844847248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,7 +1510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1309409888"/>
+        <c:crossAx val="-844851008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1801,11 +1801,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1311126080"/>
-        <c:axId val="-1349695136"/>
+        <c:axId val="-844817792"/>
+        <c:axId val="-844814032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1311126080"/>
+        <c:axId val="-844817792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.8E7"/>
@@ -1864,7 +1864,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1349695136"/>
+        <c:crossAx val="-844814032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:dispUnits>
@@ -1927,7 +1927,7 @@
         </c:dispUnits>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1349695136"/>
+        <c:axId val="-844814032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +1984,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1311126080"/>
+        <c:crossAx val="-844817792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4416,13 +4416,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O29" workbookViewId="0">
-      <selection activeCell="W53" sqref="W53"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -7727,7 +7728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>

</xml_diff>